<commit_message>
DB & FE Docker
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/프로시저 정의.xlsx
+++ b/DOC/1. 개발 문서/프로시저 정의.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8091D25E-8D61-4E6D-8956-CE29F099256C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD8C1DF-B417-4938-9608-EDCEBB61A82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2AF27EEE-D83C-44F8-BA82-F65A3019046C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>Oracle</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -85,14 +85,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"src_account_id" : "100444",
-    "dst_account_id" : "100443",
-    "dst_bank" : "1",
-    "amount" : 1000,
-    "idempotency_key" : "2" }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>/mongo/remittance/hold</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,25 +96,122 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{   "dbms": "mysql",
-    "name": "sp_remittance_hold",
-    "args": ["200039","200001","2","1000.0000","12","1"],
-    "out_count": 2 }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{ "dbms": "oracle",
-  "name": "sp_remittance_hold",
-  "args": [300791, 300001, "3", 1000, "12", "1", null, null],
-  "out_count": 2,
-  "out_types": ["number", "varchar2"] }</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{   "dbms": "postgres",
-    "name": "sp_remittance_hold",
-    "args": [400714,400004,"4","1000.0000","1","1"],
-    "mode": "func" }</t>
+    <t>"src_account_id" : "100444",
+"dst_account_id" : "100443",
+"dst_bank" : "1",
+"amount" : 1000,
+"idempotency_key" : "2"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "mysql",
+"name": "sp_remittance_hold",
+"args": ["200039","200001","2","1000.0000","12","1"],
+"out_count": 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "oracle",
+"name": "sp_remittance_hold",
+"args": [300791, 300001, "3", 1000, "12", "1", null, null],
+"out_count": 2,
+"out_types": ["number", "varchar2"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "postgres",
+"name": "sp_remittance_hold",
+"args": [400714,400004,"4","1000.0000","1","1"],
+"mode": "func"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>args</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>idempotency_key</t>
+  </si>
+  <si>
+    <t>src_account_id
+dst_account_id
+dst_bank
+amount
+idempotency_key
+type</t>
+  </si>
+  <si>
+    <t>src_account_id
+dst_account_id
+dst_bank
+amount
+idempotency_key
+type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "mysql",
+"name": "sp_receive_prepare",
+"args": ["200039","200001","2","1000.0000","12","1"],
+"out_count": 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">"dbms": "mysql",
+"name": "sp_confirm_debit_local",
+"args": ["123"],
+"out_count": 3 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">"dbms": "mysql",
+"name": "sp_confirm_credit_local",
+"args": ["1234"],
+"out_count": 3 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+"dbms": "mysql",
+"name": "sp_transfer_confirm_internal",
+"args": ["12345"],
+"out_count": 2 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "oracle",
+"name": "sp_receive_prepare",
+"args": [300791, 300001, "3", 1000, "12", "1", null, null],
+"out_count": 2,
+"out_types": ["number", "varchar2"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "oracle",
+"name": "sp_confirm_debit_local",
+"args": [123, null, null, null]
+"out_count": 3,
+"out_types": ["number", "varchar2", "varchar2"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "oracle",
+"name": "sp_remittance_hold",
+"args": [23, null, null, null]
+"out_count": 3,
+"out_types": ["number", "varchar2", "varchar2"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"dbms": "oracle",
+"name": "sp_remittance_hold",
+"args": [123, null, null
+"out_count": 2,
+"out_types": ["varchar2", "varchar2"]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>idempotency_key</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -180,7 +269,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -207,7 +296,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -219,13 +308,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -235,66 +339,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -340,9 +384,33 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -353,18 +421,68 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="medium">
@@ -376,40 +494,40 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -418,7 +536,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -429,93 +547,149 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -851,469 +1025,756 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62C3927-F370-4CCA-AF08-E319F56AA325}">
-  <dimension ref="D1:J45"/>
+  <dimension ref="D1:O45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="1.83203125" style="2" customWidth="1"/>
+    <col min="1" max="2" width="1.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.1640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="9.58203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="35.75" style="1" customWidth="1"/>
-    <col min="10" max="10" width="35.75" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.6640625" style="2"/>
+    <col min="6" max="6" width="44.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.08203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="44.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.08203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="44.83203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="16.08203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="44.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.08203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="44.83203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="16.08203125" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="4:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
+    <row r="1" spans="4:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="4:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="7"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="26" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
-    </row>
-    <row r="3" spans="4:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D3" s="34"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="11" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="28"/>
+    </row>
+    <row r="3" spans="4:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="8"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="I3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="K3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="M3" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.45">
-      <c r="D4" s="31" t="s">
+      <c r="O3" s="42" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="39"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="46"/>
+    </row>
+    <row r="5" spans="4:15" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="4"/>
+      <c r="E5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="40"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" s="16"/>
+      <c r="M5" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="48"/>
+      <c r="O5" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="10"/>
+      <c r="H6" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="4:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="29"/>
-      <c r="E5" s="15" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M6" s="35"/>
+      <c r="N6" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="20"/>
+    </row>
+    <row r="7" spans="4:15" ht="102" x14ac:dyDescent="0.45">
+      <c r="D7" s="4"/>
+      <c r="E7" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.45">
-      <c r="D6" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="15" t="s">
+      <c r="F7" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="50" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="F8" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="4:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D7" s="29"/>
-      <c r="E7" s="15" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="J8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="37"/>
+      <c r="L8" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="37"/>
+      <c r="N8" s="48" t="s">
+        <v>13</v>
+      </c>
+      <c r="O8" s="23"/>
+    </row>
+    <row r="9" spans="4:15" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="4"/>
+      <c r="E9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="8"/>
-    </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.45">
-      <c r="D8" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="F9" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="N9" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="D10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="4:10" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D9" s="29"/>
-      <c r="E9" s="15" t="s">
+      <c r="F10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="35"/>
+      <c r="N10" s="49" t="s">
+        <v>13</v>
+      </c>
+      <c r="O10" s="20"/>
+    </row>
+    <row r="11" spans="4:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D11" s="5"/>
+      <c r="E11" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.45">
-      <c r="D10" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D11" s="30"/>
-      <c r="E11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="G11" s="41"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="45"/>
+      <c r="M11" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="N11" s="51"/>
+      <c r="O11" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="O12" s="3"/>
+    </row>
+    <row r="13" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="O13" s="3"/>
+    </row>
+    <row r="14" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="O16" s="3"/>
+    </row>
+    <row r="17" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="O17" s="3"/>
+    </row>
+    <row r="18" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="O20" s="3"/>
+    </row>
+    <row r="21" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="O21" s="3"/>
+    </row>
+    <row r="22" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="O24" s="3"/>
+    </row>
+    <row r="25" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="O25" s="3"/>
+    </row>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="O28" s="3"/>
+    </row>
+    <row r="29" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="O29" s="3"/>
+    </row>
+    <row r="30" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="O30" s="3"/>
+    </row>
+    <row r="31" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="O31" s="3"/>
+    </row>
+    <row r="32" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="O32" s="3"/>
+    </row>
+    <row r="33" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="O33" s="3"/>
+    </row>
+    <row r="34" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="O34" s="3"/>
+    </row>
+    <row r="35" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="O35" s="3"/>
+    </row>
+    <row r="36" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="O36" s="3"/>
+    </row>
+    <row r="37" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="O37" s="3"/>
+    </row>
+    <row r="38" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="O38" s="3"/>
+    </row>
+    <row r="39" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="O39" s="3"/>
+    </row>
+    <row r="40" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="O40" s="3"/>
+    </row>
+    <row r="41" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
       <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="O41" s="3"/>
+    </row>
+    <row r="42" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
       <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="O42" s="3"/>
+    </row>
+    <row r="43" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
       <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="O43" s="3"/>
+    </row>
+    <row r="44" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
       <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.45">
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="O44" s="3"/>
+    </row>
+    <row r="45" spans="4:15" x14ac:dyDescent="0.45">
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
       <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="O45" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="F2:J2"/>
     <mergeCell ref="D10:D11"/>
     <mergeCell ref="D8:D9"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D2:E3"/>
+    <mergeCell ref="F2:O2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
@@ -1322,5 +1783,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RDG.py & procedure modify
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/프로시저 정의.xlsx
+++ b/DOC/1. 개발 문서/프로시저 정의.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E1299E-C1A8-4F71-9DCF-0C20791683A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33AA48D-1FB6-4785-8223-1E8B94041BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{2AF27EEE-D83C-44F8-BA82-F65A3019046C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{2AF27EEE-D83C-44F8-BA82-F65A3019046C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="33">
   <si>
     <t>Oracle</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -212,6 +212,10 @@
   </si>
   <si>
     <t>idempotency_key</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내부이체 확정에서 리턴값이 안옴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -243,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +272,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -536,7 +546,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -586,9 +596,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -655,11 +662,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -680,15 +705,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1025,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62C3927-F370-4CCA-AF08-E319F56AA325}">
-  <dimension ref="D1:O45"/>
+  <dimension ref="D1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1050,103 +1066,103 @@
     <col min="16" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="4:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="2" spans="4:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D2" s="45"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="49" t="s">
+    <row r="1" spans="4:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="4:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="51"/>
-    </row>
-    <row r="3" spans="4:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D3" s="47"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="20" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
+    </row>
+    <row r="3" spans="4:17" ht="17.5" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D3" s="52"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="31" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D4" s="44" t="s">
+    <row r="4" spans="4:17" x14ac:dyDescent="0.45">
+      <c r="D4" s="49" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="29"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="37"/>
-      <c r="O4" s="36"/>
-    </row>
-    <row r="5" spans="4:15" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D5" s="42"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="35"/>
+    </row>
+    <row r="5" spans="4:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D5" s="47"/>
       <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="30"/>
+      <c r="G5" s="29"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="24"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="9"/>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="23" t="s">
         <v>31</v>
       </c>
       <c r="L5" s="9"/>
-      <c r="M5" s="24" t="s">
+      <c r="M5" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="N5" s="38"/>
+      <c r="N5" s="37"/>
       <c r="O5" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D6" s="42" t="s">
+    <row r="6" spans="4:17" x14ac:dyDescent="0.45">
+      <c r="D6" s="47" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
@@ -1156,32 +1172,32 @@
         <v>14</v>
       </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="33" t="s">
+      <c r="H6" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="24"/>
       <c r="J6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="25"/>
+      <c r="K6" s="24"/>
       <c r="L6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="25"/>
-      <c r="N6" s="39" t="s">
+      <c r="M6" s="24"/>
+      <c r="N6" s="38" t="s">
         <v>13</v>
       </c>
       <c r="O6" s="13"/>
     </row>
-    <row r="7" spans="4:15" ht="102" x14ac:dyDescent="0.45">
-      <c r="D7" s="42"/>
+    <row r="7" spans="4:17" ht="102" x14ac:dyDescent="0.45">
+      <c r="D7" s="47"/>
       <c r="E7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>22</v>
       </c>
       <c r="H7" s="14" t="s">
@@ -1193,13 +1209,13 @@
       <c r="J7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="25" t="s">
         <v>31</v>
       </c>
       <c r="L7" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="25" t="s">
         <v>20</v>
       </c>
       <c r="N7" s="40" t="s">
@@ -1209,8 +1225,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D8" s="42" t="s">
+    <row r="8" spans="4:17" x14ac:dyDescent="0.45">
+      <c r="D8" s="47" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -1220,61 +1236,61 @@
         <v>14</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="27"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="27"/>
+      <c r="K8" s="26"/>
       <c r="L8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="27"/>
-      <c r="N8" s="38" t="s">
+      <c r="M8" s="26"/>
+      <c r="N8" s="37" t="s">
         <v>13</v>
       </c>
       <c r="O8" s="16"/>
     </row>
-    <row r="9" spans="4:15" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="D9" s="42"/>
+    <row r="9" spans="4:17" ht="97.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="D9" s="47"/>
       <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="29" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="23" t="s">
         <v>21</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="23" t="s">
         <v>31</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="24" t="s">
+      <c r="M9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="39" t="s">
         <v>30</v>
       </c>
       <c r="O9" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="4:15" x14ac:dyDescent="0.45">
-      <c r="D10" s="42" t="s">
+    <row r="10" spans="4:17" x14ac:dyDescent="0.45">
+      <c r="D10" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -1287,45 +1303,49 @@
       <c r="H10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="25"/>
+      <c r="I10" s="24"/>
       <c r="J10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="25"/>
-      <c r="N10" s="39" t="s">
+      <c r="M10" s="24"/>
+      <c r="N10" s="38" t="s">
         <v>13</v>
       </c>
       <c r="O10" s="13"/>
     </row>
-    <row r="11" spans="4:15" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="D11" s="43"/>
+    <row r="11" spans="4:17" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="D11" s="48"/>
       <c r="E11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="F11" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="28" t="s">
+      <c r="G11" s="30"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="L11" s="35"/>
-      <c r="M11" s="28" t="s">
+      <c r="L11" s="34"/>
+      <c r="M11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="N11" s="41"/>
-      <c r="O11" s="18" t="s">
+      <c r="N11" s="42"/>
+      <c r="O11" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="4:15" x14ac:dyDescent="0.45">
+      <c r="P11" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="4:17" x14ac:dyDescent="0.45">
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -1338,7 +1358,7 @@
       <c r="M12" s="3"/>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="4:17" x14ac:dyDescent="0.45">
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -1351,7 +1371,7 @@
       <c r="M13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="4:17" x14ac:dyDescent="0.45">
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
@@ -1364,7 +1384,7 @@
       <c r="M14" s="3"/>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="4:17" x14ac:dyDescent="0.45">
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -1377,7 +1397,7 @@
       <c r="M15" s="3"/>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="4:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="4:17" x14ac:dyDescent="0.45">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -1777,7 +1797,7 @@
     <mergeCell ref="D2:E3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D44:E45" xr:uid="{E9CF3308-112D-400C-95CC-E500D5C5C368}">
       <formula1>$A$4:$A$9</formula1>
     </dataValidation>

</xml_diff>